<commit_message>
Update sample download files to use consistent transaction types
Correct transaction type in sample CSV and Excel files from "withdrawal" to "withdraw" to match API expectations.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ef3a6f8e-db7d-4b32-90f3-dab5c32bf15d
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 8ae21981-532a-44ad-9ab9-3621f9b72e47
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/d2f1fa98-cfa5-41fa-9dcb-ac69ff4f4765/ef3a6f8e-db7d-4b32-90f3-dab5c32bf15d/bUOMckn
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/public/samples/sample_mixed_transactions.xlsx
+++ b/public/samples/sample_mixed_transactions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Transactions" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -438,7 +438,7 @@
         <v>02/12/2024</v>
       </c>
       <c r="C3" t="str">
-        <v>withdrawal</v>
+        <v>withdraw</v>
       </c>
       <c r="D3">
         <v>2000</v>
@@ -466,7 +466,7 @@
         <v>04/12/2024</v>
       </c>
       <c r="C5" t="str">
-        <v>withdrawal</v>
+        <v>withdraw</v>
       </c>
       <c r="D5">
         <v>1000</v>

</xml_diff>